<commit_message>
Login and shape object
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/1054/Actual/JobMaterial.xlsx
+++ b/src/test/resources/Documents/1054/Actual/JobMaterial.xlsx
@@ -71,22 +71,22 @@
     <t>Ink / Varnish</t>
   </si>
   <si>
+    <t xml:space="preserve">Black - UV - </t>
+  </si>
+  <si>
+    <t>0.28</t>
+  </si>
+  <si>
+    <t>lbs</t>
+  </si>
+  <si>
+    <t>10001817 - 9409 MIXING BLACK UV - INK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cyan - UV - </t>
   </si>
   <si>
-    <t>0.28</t>
-  </si>
-  <si>
-    <t>lbs</t>
-  </si>
-  <si>
     <t>10001837 - 9443 PRO CYAN BW8 UV - INK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black - UV - </t>
-  </si>
-  <si>
-    <t>10001817 - 9409 MIXING BLACK UV - INK</t>
   </si>
   <si>
     <t xml:space="preserve">Yellow - UV - </t>

</xml_diff>

<commit_message>
Executed for 7.1+Extent Report with docs
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/1054/Actual/JobMaterial.xlsx
+++ b/src/test/resources/Documents/1054/Actual/JobMaterial.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>Materialtype</t>
   </si>
@@ -50,19 +50,25 @@
     <t>Label  2p</t>
   </si>
   <si>
-    <t>Flexo press 4x0</t>
+    <t>Digital Print 4x0</t>
+  </si>
+  <si>
+    <t>AC505T THERMAL TRANSFER LAMINATE - 0.19 pt 11.5" 10410 ppi</t>
+  </si>
+  <si>
+    <t>555.36</t>
+  </si>
+  <si>
+    <t>M inch²</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>MATWA 1M MATTE SELF WOUND - 1.52 pt 11.25" 1310 ppi</t>
   </si>
   <si>
-    <t>598.69</t>
-  </si>
-  <si>
-    <t>M inch²</t>
-  </si>
-  <si>
-    <t/>
+    <t>543.29</t>
   </si>
   <si>
     <t>37461 - MATWA 1M MATTE SELF WOUND - 1.52 pt  1310 ppi</t>
@@ -71,34 +77,50 @@
     <t>Ink / Varnish</t>
   </si>
   <si>
-    <t xml:space="preserve">Black - UV - </t>
-  </si>
-  <si>
-    <t>0.28</t>
+    <t xml:space="preserve">Black - Digital - </t>
+  </si>
+  <si>
+    <t>0.50</t>
   </si>
   <si>
     <t>lbs</t>
   </si>
   <si>
-    <t>10001817 - 9409 MIXING BLACK UV - INK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyan - UV - </t>
-  </si>
-  <si>
-    <t>10001837 - 9443 PRO CYAN BW8 UV - INK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellow - UV - </t>
-  </si>
-  <si>
-    <t>10001305 - PROCESS YELLOW C UV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magenta - UV - </t>
-  </si>
-  <si>
-    <t>10001836 - 9442 PRO MAGENTA BW5 UV - INK</t>
+    <t>000015835 - Saphria Ink Black Labelfire UV02
+HT.400.1025/
+10L Bag In Box
+2.2lbs/Litre
+$830.00/container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow - Digital - </t>
+  </si>
+  <si>
+    <t>000015833 - Saphria Ink Yellow Labelfire UV02
+HT.400.1025/
+10L Bag In Box
+2.2lbs/Litre
+$830.00/container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyan - Digital - </t>
+  </si>
+  <si>
+    <t>000015837 - Saphria Ink Cyan Labelfire UV02
+HT.400.1025/
+10L Bag In Box
+2.2lbs/Litre
+$830.00/container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magenta - Digital - </t>
+  </si>
+  <si>
+    <t>000015831 - Saphria Ink Magenta Labelfire UV02
+HT.400.1025/
+10L Bag In Box
+2.2lbs/Litre
+$830.00/container</t>
   </si>
   <si>
     <t>Roll</t>
@@ -107,7 +129,7 @@
     <t>BOPP WHITE - 5.28 pt 11.875" 380 ppi</t>
   </si>
   <si>
-    <t>632.10</t>
+    <t>660.73</t>
   </si>
 </sst>
 </file>
@@ -115,13 +137,53 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="50">
+  <fonts count="58">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -389,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -440,6 +502,14 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -507,12 +577,12 @@
         <v>16</v>
       </c>
       <c r="H2" t="s" s="9">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="10">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s" s="11">
         <v>11</v>
@@ -521,24 +591,24 @@
         <v>12</v>
       </c>
       <c r="D3" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s" s="14">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s" s="15">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s" s="17">
         <v>19</v>
-      </c>
-      <c r="E3" t="s" s="14">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s" s="15">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s" s="16">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s" s="17">
-        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="18">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s" s="19">
         <v>11</v>
@@ -547,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="D4" t="s" s="21">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s" s="22">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s" s="23">
         <v>23</v>
-      </c>
-      <c r="E4" t="s" s="22">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s" s="23">
-        <v>21</v>
       </c>
       <c r="G4" t="s" s="24">
         <v>16</v>
@@ -564,7 +634,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="26">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s" s="27">
         <v>11</v>
@@ -576,10 +646,10 @@
         <v>25</v>
       </c>
       <c r="E5" t="s" s="30">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s" s="31">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s" s="32">
         <v>16</v>
@@ -590,7 +660,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="34">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s" s="35">
         <v>11</v>
@@ -602,10 +672,10 @@
         <v>27</v>
       </c>
       <c r="E6" t="s" s="38">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s" s="39">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s" s="40">
         <v>16</v>
@@ -616,7 +686,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="42">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s" s="43">
         <v>11</v>
@@ -625,18 +695,44 @@
         <v>12</v>
       </c>
       <c r="D7" t="s" s="45">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s" s="46">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s" s="47">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s" s="48">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s" s="49">
         <v>30</v>
       </c>
-      <c r="E7" t="s" s="46">
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="50">
         <v>31</v>
       </c>
-      <c r="F7" t="s" s="47">
+      <c r="B8" t="s" s="51">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s" s="52">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s" s="53">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s" s="54">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s" s="55">
         <v>15</v>
       </c>
-      <c r="G7" t="s" s="48">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s" s="49">
+      <c r="G8" t="s" s="56">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s" s="57">
         <v>16</v>
       </c>
     </row>

</xml_diff>